<commit_message>
fixed bugs and remade db
</commit_message>
<xml_diff>
--- a/CarPartsAccounting/Files/hello.xlsx
+++ b/CarPartsAccounting/Files/hello.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <x:si>
     <x:t>Идентификатор записи</x:t>
   </x:si>
@@ -34,25 +34,28 @@
     <x:t>2</x:t>
   </x:si>
   <x:si>
+    <x:t>Иван Петров</x:t>
+  </x:si>
+  <x:si>
+    <x:t>01.08.2020 0:00:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>15</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Выхлопная труба, Выхлопная труба, Выхлопная труба, Кузов, </x:t>
+  </x:si>
+  <x:si>
+    <x:t>4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Андрей Кругов</x:t>
+  </x:si>
+  <x:si>
     <x:t>10</x:t>
   </x:si>
   <x:si>
-    <x:t>16.07.2020 0:00:00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Андрей Круглов</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Выхлопная труба </x:t>
-  </x:si>
-  <x:si>
-    <x:t>4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>5</x:t>
-  </x:si>
-  <x:si>
-    <x:t>01.08.2020 0:00:00</x:t>
+    <x:t xml:space="preserve">Выхлопная труба, </x:t>
   </x:si>
 </x:sst>
 </file>
@@ -465,10 +468,13 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="C3" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D3" s="0" t="s">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="D3" s="0" t="s">
-        <x:v>8</x:v>
+      <x:c r="E3" s="0" t="s">
+        <x:v>13</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>